<commit_message>
Done chức năng bán hàng + ghi hoá đơn
</commit_message>
<xml_diff>
--- a/export/sanPham.xlsx
+++ b/export/sanPham.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="105">
   <si>
     <t>Mã SP</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Ảnh</t>
   </si>
   <si>
-    <t>1</t>
+    <t>111</t>
   </si>
   <si>
     <t>Pizza Hải Sản Pesto Xanh</t>
@@ -56,7 +56,7 @@
     <t>pizza0.png</t>
   </si>
   <si>
-    <t>3</t>
+    <t>112</t>
   </si>
   <si>
     <t>Pizza Hải Sản Nhiệt Đới</t>
@@ -71,7 +71,7 @@
     <t>pizza1.png</t>
   </si>
   <si>
-    <t>4</t>
+    <t>113</t>
   </si>
   <si>
     <t>Pizza Hải Sản Cocktail</t>
@@ -86,7 +86,7 @@
     <t>pizza2.png</t>
   </si>
   <si>
-    <t>5</t>
+    <t>114</t>
   </si>
   <si>
     <t>Pizza Tôm Cocktail</t>
@@ -101,7 +101,7 @@
     <t>pizza3.png</t>
   </si>
   <si>
-    <t>6</t>
+    <t>115</t>
   </si>
   <si>
     <t>Pizza Aloha</t>
@@ -113,7 +113,7 @@
     <t>pizza4.png</t>
   </si>
   <si>
-    <t>7</t>
+    <t>116</t>
   </si>
   <si>
     <t>Pizza Thịt Xông Khói</t>
@@ -125,7 +125,7 @@
     <t>pizza5.png</t>
   </si>
   <si>
-    <t>8</t>
+    <t>117</t>
   </si>
   <si>
     <t>Pizza Thịt Nguội</t>
@@ -137,7 +137,7 @@
     <t>pizza6.png</t>
   </si>
   <si>
-    <t>9</t>
+    <t>118</t>
   </si>
   <si>
     <t>Pizza Gà Nướng 3 Vị</t>
@@ -149,7 +149,7 @@
     <t>pizza7.png</t>
   </si>
   <si>
-    <t>14</t>
+    <t>119</t>
   </si>
   <si>
     <t>Pizza hải sản Pesto gấp đôi nhân</t>
@@ -161,7 +161,7 @@
     <t>pizza8.jpg</t>
   </si>
   <si>
-    <t>15</t>
+    <t>120</t>
   </si>
   <si>
     <t>Pizza gấp đôi nhân phủ cơn lốc hải sản</t>
@@ -170,7 +170,7 @@
     <t>pizza9.jpg</t>
   </si>
   <si>
-    <t>16</t>
+    <t>121</t>
   </si>
   <si>
     <t>Pizza gấp đôi nhân phủ hải sản xốt tiêu đen</t>
@@ -182,7 +182,7 @@
     <t>pizza10.jpg</t>
   </si>
   <si>
-    <t>17</t>
+    <t>122</t>
   </si>
   <si>
     <t>Pizza bò nướng tiêu đen</t>
@@ -194,7 +194,7 @@
     <t>pizza11.jpg</t>
   </si>
   <si>
-    <t>18</t>
+    <t>123</t>
   </si>
   <si>
     <t>Pizza cá ngừ thanh cua</t>
@@ -206,7 +206,7 @@
     <t>pizza12.jpg</t>
   </si>
   <si>
-    <t>33</t>
+    <t>124</t>
   </si>
   <si>
     <t>Pepsi lon 330ml</t>
@@ -218,16 +218,13 @@
     <t>19,000</t>
   </si>
   <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>Lon</t>
   </si>
   <si>
     <t>douong0.jpeg</t>
   </si>
   <si>
-    <t>34</t>
+    <t>125</t>
   </si>
   <si>
     <t>Pepsi chai 1.5l</t>
@@ -245,7 +242,7 @@
     <t>douong1.jpeg</t>
   </si>
   <si>
-    <t>35</t>
+    <t>126</t>
   </si>
   <si>
     <t>7Up lon 330ml</t>
@@ -257,7 +254,7 @@
     <t>douong2.jpeg</t>
   </si>
   <si>
-    <t>36</t>
+    <t>127</t>
   </si>
   <si>
     <t>7Up chai 1.5l</t>
@@ -269,7 +266,7 @@
     <t>douong3.jpeg</t>
   </si>
   <si>
-    <t>37</t>
+    <t>128</t>
   </si>
   <si>
     <t>Pepsi no calories 330ml</t>
@@ -281,7 +278,7 @@
     <t>douong4.jpg</t>
   </si>
   <si>
-    <t>38</t>
+    <t>129</t>
   </si>
   <si>
     <t>Mirinda cam 330ml</t>
@@ -293,9 +290,6 @@
     <t>douong5.jpg</t>
   </si>
   <si>
-    <t>39</t>
-  </si>
-  <si>
     <t>Mirinda kem soda 330ml</t>
   </si>
   <si>
@@ -305,7 +299,7 @@
     <t>douong6.jpg</t>
   </si>
   <si>
-    <t>40</t>
+    <t>131</t>
   </si>
   <si>
     <t>Nước suối Aquafina</t>
@@ -317,7 +311,7 @@
     <t>douong7.jpg</t>
   </si>
   <si>
-    <t>41</t>
+    <t>132</t>
   </si>
   <si>
     <t>Trà sữa trà đen</t>
@@ -326,19 +320,13 @@
     <t>25,000</t>
   </si>
   <si>
+    <t>25</t>
+  </si>
+  <si>
     <t>Ly</t>
   </si>
   <si>
     <t>douong8.jpg</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Trà đào cam sả</t>
-  </si>
-  <si>
-    <t>douong9.jpg</t>
   </si>
 </sst>
 </file>
@@ -426,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -777,44 +765,44 @@
         <v>67</v>
       </c>
       <c r="E15" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="F15" t="s" s="2">
+      <c r="G15" t="s" s="2">
         <v>69</v>
-      </c>
-      <c r="G15" t="s" s="2">
-        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s" s="2">
         <v>71</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>72</v>
       </c>
       <c r="C16" t="s" s="2">
         <v>66</v>
       </c>
       <c r="D16" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="E16" t="s" s="2">
+      <c r="F16" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="F16" t="s" s="2">
+      <c r="G16" t="s" s="2">
         <v>75</v>
-      </c>
-      <c r="G16" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s" s="2">
         <v>77</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>78</v>
       </c>
       <c r="C17" t="s" s="2">
         <v>66</v>
@@ -823,44 +811,44 @@
         <v>67</v>
       </c>
       <c r="E17" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F17" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s" s="2">
         <v>79</v>
-      </c>
-      <c r="F17" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="G17" t="s" s="2">
-        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s" s="2">
         <v>81</v>
-      </c>
-      <c r="B18" t="s" s="2">
-        <v>82</v>
       </c>
       <c r="C18" t="s" s="2">
         <v>66</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s" s="2">
         <v>83</v>
-      </c>
-      <c r="F18" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="G18" t="s" s="2">
-        <v>84</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s" s="2">
         <v>85</v>
-      </c>
-      <c r="B19" t="s" s="2">
-        <v>86</v>
       </c>
       <c r="C19" t="s" s="2">
         <v>66</v>
@@ -869,21 +857,21 @@
         <v>67</v>
       </c>
       <c r="E19" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s" s="2">
         <v>87</v>
-      </c>
-      <c r="F19" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="G19" t="s" s="2">
-        <v>88</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s" s="2">
         <v>89</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>90</v>
       </c>
       <c r="C20" t="s" s="2">
         <v>66</v>
@@ -892,21 +880,21 @@
         <v>67</v>
       </c>
       <c r="E20" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s" s="2">
         <v>91</v>
-      </c>
-      <c r="F20" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s" s="2">
-        <v>92</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>66</v>
@@ -915,82 +903,59 @@
         <v>67</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>66</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>66</v>
       </c>
       <c r="D23" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="E23" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="E23" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="F23" t="s" s="2">
+      <c r="G23" t="s" s="2">
         <v>104</v>
-      </c>
-      <c r="G23" t="s" s="2">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="C24" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="D24" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="E24" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="F24" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="G24" t="s" s="2">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thống kê sơ sơ
</commit_message>
<xml_diff>
--- a/export/sanPham.xlsx
+++ b/export/sanPham.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
   <si>
     <t>Mã SP</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Ảnh</t>
   </si>
   <si>
-    <t>1</t>
+    <t>67</t>
   </si>
   <si>
     <t>Pizza Hải Sản Pesto Xanh</t>
@@ -56,7 +56,7 @@
     <t>pizza0.png</t>
   </si>
   <si>
-    <t>3</t>
+    <t>68</t>
   </si>
   <si>
     <t>Pizza Hải Sản Nhiệt Đới</t>
@@ -71,7 +71,7 @@
     <t>pizza1.png</t>
   </si>
   <si>
-    <t>4</t>
+    <t>69</t>
   </si>
   <si>
     <t>Pizza Hải Sản Cocktail</t>
@@ -86,7 +86,7 @@
     <t>pizza2.png</t>
   </si>
   <si>
-    <t>5</t>
+    <t>70</t>
   </si>
   <si>
     <t>Pizza Tôm Cocktail</t>
@@ -101,7 +101,7 @@
     <t>pizza3.png</t>
   </si>
   <si>
-    <t>6</t>
+    <t>71</t>
   </si>
   <si>
     <t>Pizza Aloha</t>
@@ -113,7 +113,7 @@
     <t>pizza4.png</t>
   </si>
   <si>
-    <t>7</t>
+    <t>72</t>
   </si>
   <si>
     <t>Pizza Thịt Xông Khói</t>
@@ -125,7 +125,7 @@
     <t>pizza5.png</t>
   </si>
   <si>
-    <t>8</t>
+    <t>73</t>
   </si>
   <si>
     <t>Pizza Thịt Nguội</t>
@@ -137,208 +137,199 @@
     <t>pizza6.png</t>
   </si>
   <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>Pizza Gà Nướng 3 Vị</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>pizza7.png</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Pizza hải sản Pesto gấp đôi nhân</t>
+  </si>
+  <si>
+    <t>239,000</t>
+  </si>
+  <si>
+    <t>pizza8.jpg</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>Pizza gấp đôi nhân phủ cơn lốc hải sản</t>
+  </si>
+  <si>
+    <t>pizza9.jpg</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>Pizza gấp đôi nhân phủ hải sản xốt tiêu đen</t>
+  </si>
+  <si>
+    <t>229,000</t>
+  </si>
+  <si>
+    <t>pizza10.jpg</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>Pizza bò nướng tiêu đen</t>
+  </si>
+  <si>
+    <t>249,000</t>
+  </si>
+  <si>
+    <t>pizza11.jpg</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>Pizza cá ngừ thanh cua</t>
+  </si>
+  <si>
+    <t>269,000</t>
+  </si>
+  <si>
+    <t>pizza12.jpg</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Pepsi lon 330ml</t>
+  </si>
+  <si>
+    <t>2 - Nước uống</t>
+  </si>
+  <si>
+    <t>19,000</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>douong0.jpeg</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>Pepsi chai 1.5l</t>
+  </si>
+  <si>
+    <t>29,000</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>Chai</t>
+  </si>
+  <si>
+    <t>douong1.jpeg</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>7Up lon 330ml</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>douong2.jpeg</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>7Up chai 1.5l</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>douong3.jpeg</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>Pepsi no calories 330ml</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>douong4.jpg</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>Mirinda cam 330ml</t>
+  </si>
+  <si>
+    <t>douong5.jpg</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>Mirinda kem soda 330ml</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>douong6.jpg</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>Nước suối Aquafina</t>
+  </si>
+  <si>
+    <t>10,000</t>
+  </si>
+  <si>
+    <t>douong7.jpg</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>Trà sữa trà đen</t>
+  </si>
+  <si>
+    <t>25,000</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
-    <t>Pizza Gà Nướng 3 Vị</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>pizza7.png</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Pizza hải sản Pesto gấp đôi nhân</t>
-  </si>
-  <si>
-    <t>239,000</t>
-  </si>
-  <si>
-    <t>pizza8.jpg</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Pizza gấp đôi nhân phủ cơn lốc hải sản</t>
-  </si>
-  <si>
-    <t>pizza9.jpg</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Pizza gấp đôi nhân phủ hải sản xốt tiêu đen</t>
-  </si>
-  <si>
-    <t>229,000</t>
-  </si>
-  <si>
-    <t>pizza10.jpg</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Pizza bò nướng tiêu đen</t>
-  </si>
-  <si>
-    <t>249,000</t>
-  </si>
-  <si>
-    <t>pizza11.jpg</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Pizza cá ngừ thanh cua</t>
-  </si>
-  <si>
-    <t>269,000</t>
-  </si>
-  <si>
-    <t>pizza12.jpg</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>Pepsi lon 330ml</t>
-  </si>
-  <si>
-    <t>2 - Nước uống</t>
-  </si>
-  <si>
-    <t>19,000</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Lon</t>
-  </si>
-  <si>
-    <t>douong0.jpeg</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>Pepsi chai 1.5l</t>
-  </si>
-  <si>
-    <t>29,000</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>Chai</t>
-  </si>
-  <si>
-    <t>douong1.jpeg</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>7Up lon 330ml</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>douong2.jpeg</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>7Up chai 1.5l</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>douong3.jpeg</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Pepsi no calories 330ml</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>douong4.jpg</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>Mirinda cam 330ml</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>douong5.jpg</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>Mirinda kem soda 330ml</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>douong6.jpg</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Nước suối Aquafina</t>
-  </si>
-  <si>
-    <t>10,000</t>
-  </si>
-  <si>
-    <t>douong7.jpg</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>Trà sữa trà đen</t>
-  </si>
-  <si>
-    <t>25,000</t>
-  </si>
-  <si>
     <t>Ly</t>
   </si>
   <si>
     <t>douong8.jpg</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Trà đào cam sả</t>
-  </si>
-  <si>
-    <t>douong9.jpg</t>
   </si>
 </sst>
 </file>
@@ -426,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -892,21 +883,21 @@
         <v>67</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>69</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s" s="2">
         <v>93</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>94</v>
       </c>
       <c r="C21" t="s" s="2">
         <v>66</v>
@@ -915,82 +906,59 @@
         <v>67</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>69</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>97</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>98</v>
       </c>
       <c r="C22" t="s" s="2">
         <v>66</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s" s="2">
         <v>101</v>
-      </c>
-      <c r="B23" t="s" s="2">
-        <v>102</v>
       </c>
       <c r="C23" t="s" s="2">
         <v>66</v>
       </c>
       <c r="D23" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s" s="2">
         <v>103</v>
-      </c>
-      <c r="E23" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="F23" t="s" s="2">
         <v>104</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>105</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="B24" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="C24" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="D24" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="E24" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="F24" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="G24" t="s" s="2">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base nhẹ thống kê
</commit_message>
<xml_diff>
--- a/export/sanPham.xlsx
+++ b/export/sanPham.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="109">
   <si>
     <t>Mã SP</t>
   </si>
@@ -47,162 +47,171 @@
     <t>169,000</t>
   </si>
   <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Cái</t>
+  </si>
+  <si>
+    <t>pizza0.png</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>Pizza Hải Sản Nhiệt Đới</t>
+  </si>
+  <si>
+    <t>129,000</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>pizza1.png</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Pizza Hải Sản Cocktail</t>
+  </si>
+  <si>
+    <t>119,000</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>pizza2.png</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>Pizza Tôm Cocktail</t>
+  </si>
+  <si>
+    <t>159,000</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>pizza3.png</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>Pizza Aloha</t>
+  </si>
+  <si>
+    <t>pizza4.png</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>Pizza Thịt Xông Khói</t>
+  </si>
+  <si>
+    <t>130,000</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>pizza5.png</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>Pizza Thịt Nguội</t>
+  </si>
+  <si>
+    <t>149,000</t>
+  </si>
+  <si>
+    <t>pizza6.png</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>Pizza Gà Nướng 3 Vị</t>
+  </si>
+  <si>
     <t>43</t>
   </si>
   <si>
-    <t>Cái</t>
-  </si>
-  <si>
-    <t>pizza0.png</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>Pizza Hải Sản Nhiệt Đới</t>
-  </si>
-  <si>
-    <t>129,000</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>pizza1.png</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>Pizza Hải Sản Cocktail</t>
-  </si>
-  <si>
-    <t>119,000</t>
+    <t>pizza7.png</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>Pizza hải sản Pesto gấp đôi nhân</t>
+  </si>
+  <si>
+    <t>239,000</t>
   </si>
   <si>
     <t>48</t>
   </si>
   <si>
-    <t>pizza2.png</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>Pizza Tôm Cocktail</t>
-  </si>
-  <si>
-    <t>159,000</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>pizza3.png</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>Pizza Aloha</t>
+    <t>pizza8.jpg</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Pizza gấp đôi nhân phủ cơn lốc hải sản</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>pizza9.jpg</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>Pizza gấp đôi nhân phủ hải sản xốt tiêu đen</t>
+  </si>
+  <si>
+    <t>229,000</t>
+  </si>
+  <si>
+    <t>pizza10.jpg</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>Pizza bò nướng tiêu đen</t>
+  </si>
+  <si>
+    <t>249,000</t>
+  </si>
+  <si>
+    <t>pizza11.jpg</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Pizza cá ngừ thanh cua</t>
+  </si>
+  <si>
+    <t>269,000</t>
   </si>
   <si>
     <t>49</t>
   </si>
   <si>
-    <t>pizza4.png</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>Pizza Thịt Xông Khói</t>
-  </si>
-  <si>
-    <t>130,000</t>
-  </si>
-  <si>
-    <t>pizza5.png</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>Pizza Thịt Nguội</t>
-  </si>
-  <si>
-    <t>149,000</t>
-  </si>
-  <si>
-    <t>pizza6.png</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>Pizza Gà Nướng 3 Vị</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>pizza7.png</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>Pizza hải sản Pesto gấp đôi nhân</t>
-  </si>
-  <si>
-    <t>239,000</t>
-  </si>
-  <si>
-    <t>pizza8.jpg</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Pizza gấp đôi nhân phủ cơn lốc hải sản</t>
-  </si>
-  <si>
-    <t>pizza9.jpg</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>Pizza gấp đôi nhân phủ hải sản xốt tiêu đen</t>
-  </si>
-  <si>
-    <t>229,000</t>
-  </si>
-  <si>
-    <t>pizza10.jpg</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>Pizza bò nướng tiêu đen</t>
-  </si>
-  <si>
-    <t>249,000</t>
-  </si>
-  <si>
-    <t>pizza11.jpg</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>Pizza cá ngừ thanh cua</t>
-  </si>
-  <si>
-    <t>269,000</t>
-  </si>
-  <si>
     <t>pizza12.jpg</t>
   </si>
   <si>
@@ -233,7 +242,7 @@
     <t>29,000</t>
   </si>
   <si>
-    <t>250</t>
+    <t>248</t>
   </si>
   <si>
     <t>Chai</t>
@@ -248,7 +257,7 @@
     <t>7Up lon 330ml</t>
   </si>
   <si>
-    <t>100</t>
+    <t>84</t>
   </si>
   <si>
     <t>douong2.jpeg</t>
@@ -260,40 +269,40 @@
     <t>7Up chai 1.5l</t>
   </si>
   <si>
+    <t>douong3.jpeg</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>Pepsi no calories 330ml</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>douong4.jpg</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>Mirinda cam 330ml</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>douong5.jpg</t>
+  </si>
+  <si>
     <t>130</t>
   </si>
   <si>
-    <t>douong3.jpeg</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>Pepsi no calories 330ml</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>douong4.jpg</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>Mirinda cam 330ml</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>douong5.jpg</t>
-  </si>
-  <si>
     <t>Mirinda kem soda 330ml</t>
   </si>
   <si>
-    <t>92</t>
+    <t>85</t>
   </si>
   <si>
     <t>douong6.jpg</t>
@@ -308,6 +317,9 @@
     <t>10,000</t>
   </si>
   <si>
+    <t>59</t>
+  </si>
+  <si>
     <t>douong7.jpg</t>
   </si>
   <si>
@@ -320,7 +332,7 @@
     <t>25,000</t>
   </si>
   <si>
-    <t>25</t>
+    <t>14</t>
   </si>
   <si>
     <t>Ly</t>
@@ -558,30 +570,30 @@
         <v>21</v>
       </c>
       <c r="E6" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s" s="2">
         <v>31</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s" s="2">
-        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="C7" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="C7" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s" s="2">
+      <c r="E7" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>22</v>
       </c>
       <c r="F7" t="s" s="2">
         <v>12</v>
@@ -604,7 +616,7 @@
         <v>39</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s" s="2">
         <v>12</v>
@@ -650,21 +662,21 @@
         <v>47</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s" s="2">
         <v>12</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s" s="2">
         <v>9</v>
@@ -673,289 +685,289 @@
         <v>47</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s" s="2">
         <v>12</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>9</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s" s="2">
         <v>12</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>9</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s" s="2">
         <v>12</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s" s="2">
         <v>9</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>12</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s" s="2">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s" s="2">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s" s="2">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Xong front-end thống kê
</commit_message>
<xml_diff>
--- a/export/sanPham.xlsx
+++ b/export/sanPham.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LapTrinhJava\DoAn_QuanLyBanPizza\export\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
   <si>
     <t>Mã SP</t>
   </si>
@@ -143,7 +150,7 @@
     <t>Pizza Gà Nướng 3 Vị</t>
   </si>
   <si>
-    <t>43</t>
+    <t>42</t>
   </si>
   <si>
     <t>pizza7.png</t>
@@ -302,7 +309,7 @@
     <t>Mirinda kem soda 330ml</t>
   </si>
   <si>
-    <t>85</t>
+    <t>81</t>
   </si>
   <si>
     <t>douong6.jpg</t>
@@ -317,7 +324,7 @@
     <t>10,000</t>
   </si>
   <si>
-    <t>59</t>
+    <t>54</t>
   </si>
   <si>
     <t>douong7.jpg</t>
@@ -332,51 +339,57 @@
     <t>25,000</t>
   </si>
   <si>
-    <t>14</t>
+    <t>11</t>
   </si>
   <si>
     <t>Ly</t>
   </si>
   <si>
     <t>douong8.jpg</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>3 - Nước uống</t>
+  </si>
+  <si>
+    <t>25,001</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="9"/>
       <name val="Calibri"/>
-      <sz val="14.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
-      <sz val="13.0"/>
-      <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor indexed="17"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -384,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -393,22 +406,19 @@
       <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -416,561 +426,860 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.62109375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="46.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.28125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.4375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.90625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.3515625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="2">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="2">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="2">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s" s="2">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s" s="2">
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s" s="2">
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s" s="2">
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s" s="2">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s" s="2">
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s" s="2">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s" s="2">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s" s="2">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s" s="2">
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s" s="2">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s" s="2">
+      <c r="G6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s" s="2">
+      <c r="E7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s" s="2">
+      <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s" s="2">
+      <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
+    <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s" s="2">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s" s="2">
+      <c r="D8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s" s="2">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" t="s" s="2">
+      <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s" s="2">
+      <c r="G8" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="2">
+    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s" s="2">
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s" s="2">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s" s="2">
+      <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s" s="2">
+      <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s" s="2">
+      <c r="G9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="2">
+    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s" s="2">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s" s="2">
+      <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s" s="2">
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" t="s" s="2">
+      <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G10" t="s" s="2">
+      <c r="G10" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="2">
+    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s" s="2">
+      <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s" s="2">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s" s="2">
+      <c r="D11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s" s="2">
+      <c r="E11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F11" t="s" s="2">
+      <c r="F11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G11" t="s" s="2">
+      <c r="G11" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="2">
+    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s" s="2">
+      <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s" s="2">
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="F12" t="s" s="2">
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G12" t="s" s="2">
+      <c r="G12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="2">
+    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C13" t="s" s="2">
+      <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" t="s" s="2">
+      <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s" s="2">
+      <c r="E13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F13" t="s" s="2">
+      <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G13" t="s" s="2">
+      <c r="G13" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
+    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s" s="2">
+      <c r="B14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s" s="2">
+      <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" t="s" s="2">
+      <c r="D14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E14" t="s" s="2">
+      <c r="E14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F14" t="s" s="2">
+      <c r="F14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G14" t="s" s="2">
+      <c r="G14" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="2">
+    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" t="s" s="2">
+      <c r="B15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C15" t="s" s="2">
+      <c r="C15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s" s="2">
+      <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E15" t="s" s="2">
+      <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" t="s" s="2">
+      <c r="F15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G15" t="s" s="2">
+      <c r="G15" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="2">
+    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" t="s" s="2">
+      <c r="B16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C16" t="s" s="2">
+      <c r="C16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="s" s="2">
+      <c r="D16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E16" t="s" s="2">
+      <c r="E16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F16" t="s" s="2">
+      <c r="F16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G16" t="s" s="2">
+      <c r="G16" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="2">
+    <row r="17" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="B17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C17" t="s" s="2">
+      <c r="C17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D17" t="s" s="2">
+      <c r="D17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E17" t="s" s="2">
+      <c r="E17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F17" t="s" s="2">
+      <c r="F17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G17" t="s" s="2">
+      <c r="G17" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="2">
+    <row r="18" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="B18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C18" t="s" s="2">
+      <c r="C18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D18" t="s" s="2">
+      <c r="D18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E18" t="s" s="2">
+      <c r="E18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F18" t="s" s="2">
+      <c r="F18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G18" t="s" s="2">
+      <c r="G18" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="2">
+    <row r="19" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s" s="2">
+      <c r="C19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D19" t="s" s="2">
+      <c r="D19" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E19" t="s" s="2">
+      <c r="E19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F19" t="s" s="2">
+      <c r="F19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G19" t="s" s="2">
+      <c r="G19" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="2">
+    <row r="20" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s" s="2">
+      <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s" s="2">
+      <c r="C20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D20" t="s" s="2">
+      <c r="D20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E20" t="s" s="2">
+      <c r="E20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F20" t="s" s="2">
+      <c r="F20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G20" t="s" s="2">
+      <c r="G20" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="2">
+    <row r="21" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B21" t="s" s="2">
+      <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C21" t="s" s="2">
+      <c r="C21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D21" t="s" s="2">
+      <c r="D21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E21" t="s" s="2">
+      <c r="E21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F21" t="s" s="2">
+      <c r="F21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G21" t="s" s="2">
+      <c r="G21" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="2">
+    <row r="22" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B22" t="s" s="2">
+      <c r="B22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C22" t="s" s="2">
+      <c r="C22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D22" t="s" s="2">
+      <c r="D22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E22" t="s" s="2">
+      <c r="E22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F22" t="s" s="2">
+      <c r="F22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G22" t="s" s="2">
+      <c r="G22" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="2">
+    <row r="23" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B23" t="s" s="2">
+      <c r="B23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C23" t="s" s="2">
+      <c r="C23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D23" t="s" s="2">
+      <c r="D23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E23" t="s" s="2">
+      <c r="E23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F23" t="s" s="2">
+      <c r="F23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G23" t="s" s="2">
+      <c r="G23" s="2" t="s">
         <v>108</v>
       </c>
     </row>
+    <row r="24" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>